<commit_message>
Reformatted code and separated the text part of the greetings
</commit_message>
<xml_diff>
--- a/Greetings.xlsx
+++ b/Greetings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerome\AndroidStudioProjects\greetings_singapore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04907CA2-4580-4B7C-A5FB-F0A3C715CB38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4209D2-58A1-490A-8DC1-3B946676D96F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{5EC5286B-CD0E-469A-918D-ED59DD4B17FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5EC5286B-CD0E-469A-918D-ED59DD4B17FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blessing" sheetId="1" r:id="rId1"/>
@@ -843,10 +843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8832A0-1090-4F4A-9A85-7E5DCBB5DD32}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -854,7 +854,7 @@
     <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>